<commit_message>
more work on firmware, electrodes work
</commit_message>
<xml_diff>
--- a/NextFlex/BOM_REV_B.xlsx
+++ b/NextFlex/BOM_REV_B.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -163,6 +163,27 @@
   <si>
     <t xml:space="preserve">C112161</t>
   </si>
+  <si>
+    <t xml:space="preserve">Green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D3, D5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED_0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C72043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D4, D7, D8, D9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2286</t>
+  </si>
 </sst>
 </file>
 
@@ -436,8 +457,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -607,16 +628,32 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+      <c r="A12" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
+      <c r="A13" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="16"/>
@@ -628,7 +665,7 @@
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
+      <c r="D15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="16"/>

</xml_diff>

<commit_message>
place final revision order for next flex
</commit_message>
<xml_diff>
--- a/NextFlex/BOM_REV_B.xlsx
+++ b/NextFlex/BOM_REV_B.xlsx
@@ -86,7 +86,7 @@
     <t xml:space="preserve">1uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C1, C2, C7, C8. C10, C11, C12</t>
+    <t xml:space="preserve">C1, C2, C7, C8, C10, C11, C12</t>
   </si>
   <si>
     <t xml:space="preserve"> C15849</t>
@@ -458,7 +458,7 @@
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>